<commit_message>
Update code for compile data + clustering + linear regression
</commit_message>
<xml_diff>
--- a/Input/selection_indicators_immigration.xlsx
+++ b/Input/selection_indicators_immigration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\github\Immigration_causes\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F55F87-5CFE-4C06-B6D6-8DEFBFC3EC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3E823E-497C-429A-A7BA-5DF3E2014BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D79B3A47-F2A5-40C7-B014-0523F94630AA}"/>
   </bookViews>
@@ -9435,8 +9435,8 @@
   <dimension ref="A1:I1489"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A1062" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1082" sqref="D1082"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9502,7 +9502,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -10133,7 +10133,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -10147,7 +10147,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -10495,7 +10495,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -10551,7 +10551,7 @@
         <v>2986</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -10601,7 +10601,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>240</v>
       </c>
@@ -11037,7 +11037,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>272</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>330</v>
       </c>
@@ -11481,7 +11481,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>350</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>452</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>468</v>
       </c>
@@ -12214,7 +12214,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>480</v>
       </c>
@@ -12294,7 +12294,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>494</v>
       </c>
@@ -12864,7 +12864,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>596</v>
       </c>
@@ -13181,7 +13181,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>652</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>676</v>
       </c>
@@ -13418,7 +13418,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>694</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>702</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>782</v>
       </c>
@@ -13925,7 +13925,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>784</v>
       </c>
@@ -13939,7 +13939,7 @@
         <v>2984</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>786</v>
       </c>
@@ -14317,7 +14317,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>852</v>
       </c>
@@ -14825,7 +14825,7 @@
         <v>2983</v>
       </c>
     </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>940</v>
       </c>
@@ -14894,7 +14894,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>952</v>
       </c>
@@ -14908,7 +14908,7 @@
         <v>2986</v>
       </c>
     </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>954</v>
       </c>
@@ -14966,7 +14966,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="484" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>964</v>
       </c>
@@ -16084,7 +16084,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="584" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A584" t="s">
         <v>1164</v>
       </c>
@@ -16560,7 +16560,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="627" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="627" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
         <v>1250</v>
       </c>
@@ -16676,7 +16676,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="637" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="637" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>1270</v>
       </c>
@@ -16767,7 +16767,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="645" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="645" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A645" t="s">
         <v>1286</v>
       </c>
@@ -17367,7 +17367,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="699" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="699" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A699" t="s">
         <v>1394</v>
       </c>
@@ -17458,7 +17458,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="707" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="707" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A707" t="s">
         <v>1410</v>
       </c>
@@ -17472,7 +17472,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="708" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A708" t="s">
         <v>1412</v>
       </c>
@@ -17486,7 +17486,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="709" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="709" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A709" t="s">
         <v>1414</v>
       </c>
@@ -17500,7 +17500,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="710" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="710" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A710" t="s">
         <v>1416</v>
       </c>
@@ -17514,7 +17514,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="711" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A711" t="s">
         <v>1418</v>
       </c>
@@ -18340,7 +18340,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="785" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="785" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
         <v>1566</v>
       </c>
@@ -18409,7 +18409,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="791" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="791" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
         <v>1578</v>
       </c>
@@ -20296,7 +20296,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="962" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="962" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A962" t="s">
         <v>1920</v>
       </c>
@@ -20420,7 +20420,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="973" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="973" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A973" t="s">
         <v>1942</v>
       </c>
@@ -20456,7 +20456,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="976" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="976" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A976" t="s">
         <v>1948</v>
       </c>
@@ -20558,7 +20558,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="985" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="985" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A985" t="s">
         <v>1966</v>
       </c>
@@ -20759,7 +20759,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1003" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1003" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1003" t="s">
         <v>2002</v>
       </c>
@@ -20930,7 +20930,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1018" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1018" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
         <v>2032</v>
       </c>
@@ -20944,7 +20944,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1019" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1019" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
         <v>2034</v>
       </c>
@@ -20958,7 +20958,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1020" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1020" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
         <v>2036</v>
       </c>
@@ -20972,7 +20972,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1021" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1021" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
         <v>2038</v>
       </c>
@@ -20986,7 +20986,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1022" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1022" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1022" t="s">
         <v>2040</v>
       </c>
@@ -21000,7 +21000,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1023" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1023" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1023" t="s">
         <v>2042</v>
       </c>
@@ -21014,7 +21014,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1024" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1024" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1024" t="s">
         <v>2044</v>
       </c>
@@ -21028,7 +21028,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1025" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1025" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1025" t="s">
         <v>2046</v>
       </c>
@@ -21042,7 +21042,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1026" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1026" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1026" t="s">
         <v>2048</v>
       </c>
@@ -21056,7 +21056,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1027" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1027" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1027" t="s">
         <v>2050</v>
       </c>
@@ -21070,7 +21070,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1028" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1028" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1028" t="s">
         <v>2052</v>
       </c>
@@ -21084,7 +21084,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1029" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1029" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1029" t="s">
         <v>2054</v>
       </c>
@@ -21098,7 +21098,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1030" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1030" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1030" t="s">
         <v>2056</v>
       </c>
@@ -21112,7 +21112,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1031" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1031" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1031" t="s">
         <v>2058</v>
       </c>
@@ -21126,7 +21126,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1032" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1032" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1032" t="s">
         <v>2060</v>
       </c>
@@ -21140,7 +21140,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1033" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1033" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1033" t="s">
         <v>2062</v>
       </c>
@@ -21154,7 +21154,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1034" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1034" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1034" t="s">
         <v>2064</v>
       </c>
@@ -21168,7 +21168,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1035" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1035" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1035" t="s">
         <v>2066</v>
       </c>
@@ -21182,7 +21182,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1036" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1036" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1036" t="s">
         <v>2068</v>
       </c>
@@ -21196,7 +21196,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1037" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1037" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1037" t="s">
         <v>2070</v>
       </c>
@@ -21210,7 +21210,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1038" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1038" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1038" t="s">
         <v>2072</v>
       </c>
@@ -21224,7 +21224,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1039" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1039" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1039" t="s">
         <v>2074</v>
       </c>
@@ -21238,7 +21238,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1040" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1040" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1040" t="s">
         <v>2076</v>
       </c>
@@ -21252,7 +21252,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1041" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1041" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1041" t="s">
         <v>2078</v>
       </c>
@@ -21266,7 +21266,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1042" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1042" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1042" t="s">
         <v>2080</v>
       </c>
@@ -21280,7 +21280,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1043" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1043" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1043" t="s">
         <v>2082</v>
       </c>
@@ -21294,7 +21294,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1044" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1044" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1044" t="s">
         <v>2084</v>
       </c>
@@ -21308,7 +21308,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1045" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1045" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1045" t="s">
         <v>2086</v>
       </c>
@@ -21322,7 +21322,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1046" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1046" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1046" t="s">
         <v>2088</v>
       </c>
@@ -21336,7 +21336,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1047" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1047" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1047" t="s">
         <v>2090</v>
       </c>
@@ -21350,7 +21350,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1048" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1048" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1048" t="s">
         <v>2092</v>
       </c>
@@ -21364,7 +21364,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1049" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1049" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1049" t="s">
         <v>2094</v>
       </c>
@@ -21378,7 +21378,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1050" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1050" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1050" t="s">
         <v>2096</v>
       </c>
@@ -21392,7 +21392,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1051" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1051" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1051" t="s">
         <v>2098</v>
       </c>
@@ -21406,7 +21406,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1052" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1052" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1052" t="s">
         <v>2100</v>
       </c>
@@ -21420,7 +21420,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1053" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1053" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1053" t="s">
         <v>2102</v>
       </c>
@@ -21434,7 +21434,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1054" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1054" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1054" t="s">
         <v>2104</v>
       </c>
@@ -21448,7 +21448,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1055" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1055" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1055" t="s">
         <v>2106</v>
       </c>
@@ -21462,7 +21462,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1056" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1056" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1056" t="s">
         <v>2108</v>
       </c>
@@ -21476,7 +21476,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1057" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1057" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1057" t="s">
         <v>2110</v>
       </c>
@@ -21490,7 +21490,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1058" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1058" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1058" t="s">
         <v>2112</v>
       </c>
@@ -21504,7 +21504,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1059" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1059" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1059" t="s">
         <v>2114</v>
       </c>
@@ -21518,7 +21518,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1060" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1060" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1060" t="s">
         <v>2116</v>
       </c>
@@ -21532,7 +21532,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1061" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1061" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1061" t="s">
         <v>2118</v>
       </c>
@@ -21546,7 +21546,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1062" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1062" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1062" t="s">
         <v>2120</v>
       </c>
@@ -21560,7 +21560,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1063" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1063" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1063" t="s">
         <v>2122</v>
       </c>
@@ -21574,7 +21574,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1064" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1064" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1064" t="s">
         <v>2124</v>
       </c>
@@ -21588,7 +21588,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1065" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1065" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1065" t="s">
         <v>2126</v>
       </c>
@@ -21602,7 +21602,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1066" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1066" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1066" t="s">
         <v>2128</v>
       </c>
@@ -21616,7 +21616,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1067" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1067" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1067" t="s">
         <v>2130</v>
       </c>
@@ -21630,7 +21630,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1068" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1068" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1068" t="s">
         <v>2132</v>
       </c>
@@ -21644,7 +21644,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1069" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1069" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1069" t="s">
         <v>2134</v>
       </c>
@@ -21658,7 +21658,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1070" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1070" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1070" t="s">
         <v>2136</v>
       </c>
@@ -21672,7 +21672,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1071" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1071" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1071" t="s">
         <v>2138</v>
       </c>
@@ -21697,7 +21697,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1073" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1073" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1073" t="s">
         <v>2142</v>
       </c>
@@ -21722,7 +21722,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1075" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1075" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1075" t="s">
         <v>2146</v>
       </c>
@@ -21736,7 +21736,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1076" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1076" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1076" t="s">
         <v>2148</v>
       </c>
@@ -21750,7 +21750,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1077" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1077" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1077" t="s">
         <v>2150</v>
       </c>
@@ -21808,7 +21808,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1082" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1082" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1082" t="s">
         <v>2160</v>
       </c>
@@ -21816,7 +21816,7 @@
         <v>2161</v>
       </c>
       <c r="C1082" t="s">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="D1082" t="s">
         <v>2985</v>
@@ -21888,7 +21888,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1089" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1089" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1089" t="s">
         <v>2174</v>
       </c>
@@ -21902,7 +21902,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1090" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1090" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1090" t="s">
         <v>2176</v>
       </c>
@@ -21916,7 +21916,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1091" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1091" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1091" t="s">
         <v>2178</v>
       </c>
@@ -21930,7 +21930,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1092" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1092" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1092" t="s">
         <v>2180</v>
       </c>
@@ -22615,7 +22615,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1154" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1154" t="s">
         <v>2304</v>
       </c>
@@ -22629,7 +22629,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1155" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1155" t="s">
         <v>2306</v>
       </c>
@@ -22643,7 +22643,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1156" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1156" t="s">
         <v>2308</v>
       </c>
@@ -22657,7 +22657,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1157" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1157" t="s">
         <v>2310</v>
       </c>
@@ -22737,7 +22737,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1164" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1164" t="s">
         <v>2324</v>
       </c>
@@ -23539,7 +23539,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1235" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1235" t="s">
         <v>2466</v>
       </c>
@@ -23553,7 +23553,7 @@
         <v>2985</v>
       </c>
     </row>
-    <row r="1236" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1236" t="s">
         <v>2468</v>
       </c>
@@ -25074,7 +25074,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1374" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1374" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1374" t="s">
         <v>2744</v>
       </c>
@@ -25198,7 +25198,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1385" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1385" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1385" t="s">
         <v>2766</v>
       </c>
@@ -25843,7 +25843,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1442" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1442" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A1442" t="s">
         <v>2880</v>
       </c>
@@ -25989,7 +25989,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1455" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1455" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1455" t="s">
         <v>2906</v>
       </c>
@@ -26267,7 +26267,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1480" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1480" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1480" t="s">
         <v>2956</v>
       </c>
@@ -26336,7 +26336,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="1486" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="1486" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1486" t="s">
         <v>2968</v>
       </c>
@@ -26387,7 +26387,12 @@
   <autoFilter ref="A1:D1489" xr:uid="{52EAD19D-1550-4E26-88DB-9A24B2659495}">
     <filterColumn colId="2">
       <filters>
-        <filter val="y"/>
+        <filter val="n"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="population"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>